<commit_message>
wind_port column name correction
changed column name in wind port dataset that was unreadable by r
</commit_message>
<xml_diff>
--- a/data-raw/SoE_EJ_2024_Final.xlsx
+++ b/data-raw/SoE_EJ_2024_Final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angela.silva\Documents\Wind\SOE\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon.beltz\Documents\GitHub\ecodata\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,9 +41,6 @@
     <t>MAX_%val</t>
   </si>
   <si>
-    <t>MAX_$val</t>
-  </si>
-  <si>
     <t>EJ</t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>count_yrs</t>
+  </si>
+  <si>
+    <t>MaxVal</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,27 +641,27 @@
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>6.0018510661753441E-2</v>
@@ -688,10 +688,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
         <v>0.16358492179019093</v>
@@ -718,10 +718,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>0.10229498874489337</v>
@@ -748,10 +748,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
         <v>6.2298666228713016E-2</v>
@@ -778,10 +778,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
         <v>5.7839849803637565E-2</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>4.5703807472212928E-2</v>
@@ -834,10 +834,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
         <v>2.2411139177219604E-2</v>
@@ -864,10 +864,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <v>5.1119198238275411E-2</v>
@@ -896,10 +896,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2">
         <v>7.0251122860580092E-2</v>
@@ -926,10 +926,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
         <v>2.7338673131735221E-2</v>
@@ -956,10 +956,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2">
         <v>2.6109165101670235E-2</v>
@@ -986,10 +986,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <v>2.2982931145233351E-2</v>
@@ -1018,10 +1018,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2">
         <v>9.754947355646984E-2</v>
@@ -1046,10 +1046,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2">
         <v>5.7265458027157851E-2</v>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2">
         <v>1.2011098903760791E-2</v>
@@ -1104,10 +1104,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2">
         <v>1.31003161766194E-2</v>
@@ -1134,10 +1134,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="2">
         <v>3.1989405387614675E-2</v>
@@ -1166,10 +1166,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="2">
         <v>9.9129396724979245E-3</v>
@@ -1196,10 +1196,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="2">
         <v>5.3831280514968676E-3</v>
@@ -1228,10 +1228,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2">
         <v>1.7447323168845758E-2</v>
@@ -1258,10 +1258,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2">
         <v>8.9675073468603612E-3</v>
@@ -1288,10 +1288,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="2">
         <v>3.1515441701231717E-2</v>
@@ -1320,10 +1320,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="2">
         <v>0.13769602022801528</v>
@@ -1348,10 +1348,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2">
         <v>0.28718276567960771</v>
@@ -1380,10 +1380,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" s="2">
         <v>5.2069203685740868E-2</v>
@@ -1410,10 +1410,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="2">
         <v>0.16429196708427779</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="2">
         <v>8.7222088259322067E-2</v>
@@ -1470,10 +1470,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" s="2">
         <v>0.22564969370646876</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2">
         <v>5.4437501353278454E-2</v>
@@ -1532,10 +1532,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31" s="2">
         <v>3.2828154127135148E-2</v>
@@ -1560,10 +1560,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32" s="2">
         <v>2.0026029839631896E-2</v>
@@ -1588,10 +1588,10 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33" s="2">
         <v>3.0462138623852018E-2</v>
@@ -1618,10 +1618,10 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34" s="2">
         <v>0.15708091582193534</v>
@@ -1646,10 +1646,10 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C35" s="2">
         <v>0.16022264746132886</v>
@@ -1676,10 +1676,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2">
         <v>1.6306219317906108E-2</v>
@@ -1704,10 +1704,10 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C37" s="2">
         <v>1.3247760280930823E-2</v>
@@ -1734,10 +1734,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38" s="2">
         <v>3.2033556867838889E-2</v>
@@ -1762,10 +1762,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" s="2">
         <v>2.2697055193572652E-2</v>
@@ -1792,10 +1792,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C40" s="2">
         <v>1.5467419642254213E-2</v>
@@ -1822,10 +1822,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C41" s="2">
         <v>6.8724800692205226E-2</v>
@@ -1850,10 +1850,10 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" s="2">
         <v>7.3616345259542762E-2</v>
@@ -1880,10 +1880,10 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C43" s="2">
         <v>2.1719059269325599E-2</v>
@@ -1910,10 +1910,10 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C44" s="2">
         <v>9.5609395301352665E-2</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45" s="2">
         <v>0.11089864739523338</v>
@@ -1970,10 +1970,10 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C46" s="2">
         <v>2.5968775076037068E-2</v>
@@ -2000,10 +2000,10 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C47" s="2">
         <v>6.9141628218834614E-2</v>
@@ -2030,10 +2030,10 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C48" s="2">
         <v>6.8136796670095374E-3</v>
@@ -2060,10 +2060,10 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C49" s="2">
         <v>1.7443018547321859E-2</v>
@@ -2090,10 +2090,10 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C50" s="2">
         <v>1.3135317112751748E-2</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C51" s="2">
         <v>3.119738882086377E-3</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C52" s="2">
         <v>5.7041229516436656E-3</v>
@@ -2178,10 +2178,10 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C53" s="2">
         <v>5.7208597107864436E-3</v>
@@ -2208,10 +2208,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C54" s="2">
         <v>3.6973572608621818E-3</v>

</xml_diff>